<commit_message>
Corrects the tel scheme USSD test result for iOS Gmail tfrom none to blocked
</commit_message>
<xml_diff>
--- a/[03] Evaluation/Evaluation.xlsx
+++ b/[03] Evaluation/Evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinbaechle/Library/Mobile Documents/com~apple~CloudDocs/[02] Uni/[01] KIT/[01] Module/[02] Informatik/Informationssicherheit/Praktikum Security, Usability and Society/EML-Files/[03] Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A11AC8-DC70-6941-B594-64C75C97402E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D7B07A-9C36-B84C-9FA9-D265F316F080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{0F2F2031-B468-514E-8318-7BA7EB2FC991}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{0F2F2031-B468-514E-8318-7BA7EB2FC991}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="9" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="33" r:id="rId10"/>
+    <pivotCache cacheId="34" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1186,7 +1186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1320,7 +1320,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -11949,7 +11948,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{015AA2D7-3D90-D349-B341-03E2450F3305}" name="PivotTable2" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{015AA2D7-3D90-D349-B341-03E2450F3305}" name="PivotTable2" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A35:B49" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -12067,7 +12066,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6AEAD8A6-5E60-0F43-97B0-5793E6ED493D}" name="PivotTable1" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6AEAD8A6-5E60-0F43-97B0-5793E6ED493D}" name="PivotTable1" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -12147,7 +12146,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E185F0B5-6C55-6F48-9917-5A22208D1E4B}" name="PivotTable6" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E185F0B5-6C55-6F48-9917-5A22208D1E4B}" name="PivotTable6" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A137:B146" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -12341,7 +12340,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C78F983C-F91D-D541-B4A8-1B2773E2941C}" name="PivotTable5" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C78F983C-F91D-D541-B4A8-1B2773E2941C}" name="PivotTable5" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A118:B123" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -12464,7 +12463,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FCDF445C-B99D-264A-B82D-C1C5AA72098E}" name="PivotTable4" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FCDF445C-B99D-264A-B82D-C1C5AA72098E}" name="PivotTable4" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A81:A112" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -12633,7 +12632,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2E23E819-2EDC-5C46-A5EE-5A8BEEC7F066}" name="PivotTable3" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2E23E819-2EDC-5C46-A5EE-5A8BEEC7F066}" name="PivotTable3" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A62:F72" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0">
@@ -12835,14 +12834,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7676E655-0B6C-AF42-ADF8-BCD3155B7F32}" name="EvidenceEvaluation" displayName="EvidenceEvaluation" ref="A1:K217" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:K217" xr:uid="{7676E655-0B6C-AF42-ADF8-BCD3155B7F32}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Android_Proton"/>
-        <filter val="iOS_Proton"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K217" xr:uid="{7676E655-0B6C-AF42-ADF8-BCD3155B7F32}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K217">
     <sortCondition descending="1" ref="B1:B217"/>
   </sortState>
@@ -12902,7 +12894,7 @@
   <autoFilter ref="A1:B4" xr:uid="{91B26C6F-9BA3-614E-99FD-6502CAA11081}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4703EAF9-0CEE-FB4A-9171-08B43E9BDD80}" name="support"/>
-    <tableColumn id="2" xr3:uid="{88D5354A-6643-6745-879D-E0F8BB71D41F}" name="description" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{88D5354A-6643-6745-879D-E0F8BB71D41F}" name="description" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12913,7 +12905,7 @@
   <autoFilter ref="A1:B6" xr:uid="{AFB7D28E-8B5A-5142-BEFE-FC4C555A1A08}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D6A47748-9FAB-6A46-9516-F3AB885A9B8B}" name="interaction"/>
-    <tableColumn id="2" xr3:uid="{D9DAC3F6-8DDD-D040-8C38-E06C98559E85}" name="description" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{D9DAC3F6-8DDD-D040-8C38-E06C98559E85}" name="description" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13249,8 +13241,8 @@
   </sheetPr>
   <dimension ref="B1:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:E21"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14311,8 +14303,8 @@
   </sheetPr>
   <dimension ref="A1:K221"/>
   <sheetViews>
-    <sheetView topLeftCell="B27" zoomScale="75" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27:I90"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="75" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14364,7 +14356,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -14394,14 +14386,14 @@
         <v>4</v>
       </c>
       <c r="J2" s="2" t="str">
-        <f>$F2&amp;"."&amp;$G2&amp;"."&amp;$H2</f>
+        <f t="shared" ref="J2:J33" si="0">$F2&amp;"."&amp;$G2&amp;"."&amp;$H2</f>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
@@ -14431,7 +14423,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f>$F3&amp;"."&amp;$G3&amp;"."&amp;$H3</f>
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -14468,14 +14460,14 @@
         <v>4</v>
       </c>
       <c r="J4" s="2" t="str">
-        <f>$F4&amp;"."&amp;$G4&amp;"."&amp;$H4</f>
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -14505,14 +14497,14 @@
         <v>4</v>
       </c>
       <c r="J5" s="2" t="str">
-        <f>$F5&amp;"."&amp;$G5&amp;"."&amp;$H5</f>
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -14542,14 +14534,14 @@
         <v>4</v>
       </c>
       <c r="J6" s="2" t="str">
-        <f>$F6&amp;"."&amp;$G6&amp;"."&amp;$H6</f>
+        <f t="shared" si="0"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
@@ -14579,14 +14571,14 @@
         <v>4</v>
       </c>
       <c r="J7" s="2" t="str">
-        <f>$F7&amp;"."&amp;$G7&amp;"."&amp;$H7</f>
+        <f t="shared" si="0"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -14616,7 +14608,7 @@
         <v>4</v>
       </c>
       <c r="J8" s="2" t="str">
-        <f>$F8&amp;"."&amp;$G8&amp;"."&amp;$H8</f>
+        <f t="shared" si="0"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -14624,13 +14616,13 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="58" t="s">
@@ -14639,28 +14631,28 @@
       <c r="E9" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="65" t="s">
+      <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="65" t="s">
+      <c r="G9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="65">
+      <c r="I9" s="2">
         <f>IFERROR(INT(IF($J9=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J9=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J9=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J9=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J9=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J9=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J9=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J9=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J9=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J9=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J9=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J9=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J9=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J9=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J9=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J9=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J9=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J9=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J9=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J9=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J9=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J9=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J9=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J9=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J9=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J9=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J9=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>4</v>
       </c>
-      <c r="J9" s="65" t="str">
-        <f>$F9&amp;"."&amp;$G9&amp;"."&amp;$H9</f>
+      <c r="J9" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
-      <c r="K9" s="65" t="s">
+      <c r="K9" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>37</v>
       </c>
@@ -14690,14 +14682,14 @@
         <v>4</v>
       </c>
       <c r="J10" s="14" t="str">
-        <f>$F10&amp;"."&amp;$G10&amp;"."&amp;$H10</f>
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
@@ -14727,7 +14719,7 @@
         <v>4</v>
       </c>
       <c r="J11" s="2" t="str">
-        <f>$F11&amp;"."&amp;$G11&amp;"."&amp;$H11</f>
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -14764,14 +14756,14 @@
         <v>4</v>
       </c>
       <c r="J12" s="2" t="str">
-        <f>$F12&amp;"."&amp;$G12&amp;"."&amp;$H12</f>
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -14801,14 +14793,14 @@
         <v>4</v>
       </c>
       <c r="J13" s="2" t="str">
-        <f>$F13&amp;"."&amp;$G13&amp;"."&amp;$H13</f>
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -14838,14 +14830,14 @@
         <v>4</v>
       </c>
       <c r="J14" s="2" t="str">
-        <f>$F14&amp;"."&amp;$G14&amp;"."&amp;$H14</f>
+        <f t="shared" si="0"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
@@ -14875,14 +14867,14 @@
         <v>4</v>
       </c>
       <c r="J15" s="2" t="str">
-        <f>$F15&amp;"."&amp;$G15&amp;"."&amp;$H15</f>
+        <f t="shared" si="0"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
@@ -14912,7 +14904,7 @@
         <v>4</v>
       </c>
       <c r="J16" s="2" t="str">
-        <f>$F16&amp;"."&amp;$G16&amp;"."&amp;$H16</f>
+        <f t="shared" si="0"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -14920,13 +14912,13 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="65" t="s">
+      <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="65" t="s">
+      <c r="B17" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C17" s="65" t="s">
+      <c r="C17" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="58" t="s">
@@ -14935,28 +14927,28 @@
       <c r="E17" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="65" t="s">
+      <c r="F17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="65" t="s">
+      <c r="G17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="65">
+      <c r="I17" s="2">
         <f>IFERROR(INT(IF($J17=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J17=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J17=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J17=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J17=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J17=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J17=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J17=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J17=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J17=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J17=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J17=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J17=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J17=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J17=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J17=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J17=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J17=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J17=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J17=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J17=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J17=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J17=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J17=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J17=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J17=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J17=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>4</v>
       </c>
-      <c r="J17" s="65" t="str">
-        <f>$F17&amp;"."&amp;$G17&amp;"."&amp;$H17</f>
+      <c r="J17" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
-      <c r="K17" s="65" t="s">
+      <c r="K17" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>37</v>
       </c>
@@ -14986,14 +14978,14 @@
         <v>4</v>
       </c>
       <c r="J18" s="14" t="str">
-        <f>$F18&amp;"."&amp;$G18&amp;"."&amp;$H18</f>
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K18" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
@@ -15023,7 +15015,7 @@
         <v>4</v>
       </c>
       <c r="J19" s="2" t="str">
-        <f>$F19&amp;"."&amp;$G19&amp;"."&amp;$H19</f>
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -15060,14 +15052,14 @@
         <v>4</v>
       </c>
       <c r="J20" s="2" t="str">
-        <f>$F20&amp;"."&amp;$G20&amp;"."&amp;$H20</f>
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
@@ -15097,14 +15089,14 @@
         <v>4</v>
       </c>
       <c r="J21" s="2" t="str">
-        <f>$F21&amp;"."&amp;$G21&amp;"."&amp;$H21</f>
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
@@ -15134,14 +15126,14 @@
         <v>4</v>
       </c>
       <c r="J22" s="2" t="str">
-        <f>$F22&amp;"."&amp;$G22&amp;"."&amp;$H22</f>
+        <f t="shared" si="0"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
@@ -15171,14 +15163,14 @@
         <v>4</v>
       </c>
       <c r="J23" s="2" t="str">
-        <f>$F23&amp;"."&amp;$G23&amp;"."&amp;$H23</f>
+        <f t="shared" si="0"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
@@ -15208,7 +15200,7 @@
         <v>4</v>
       </c>
       <c r="J24" s="2" t="str">
-        <f>$F24&amp;"."&amp;$G24&amp;"."&amp;$H24</f>
+        <f t="shared" si="0"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K24" s="2" t="s">
@@ -15216,13 +15208,13 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="65" t="s">
+      <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="65" t="s">
+      <c r="B25" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C25" s="65" t="s">
+      <c r="C25" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D25" s="57" t="s">
@@ -15231,28 +15223,28 @@
       <c r="E25" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="65" t="s">
+      <c r="F25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G25" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25" s="65" t="s">
+      <c r="G25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I25" s="65">
+      <c r="I25" s="2">
         <f>IFERROR(INT(IF($J25=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J25=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J25=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J25=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J25=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J25=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J25=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J25=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J25=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J25=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J25=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J25=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J25=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J25=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J25=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J25=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J25=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J25=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J25=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J25=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J25=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J25=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J25=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J25=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J25=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J25=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J25=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>4</v>
       </c>
-      <c r="J25" s="65" t="str">
-        <f>$F25&amp;"."&amp;$G25&amp;"."&amp;$H25</f>
+      <c r="J25" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>both.none.yes_misleading-first</v>
       </c>
-      <c r="K25" s="65" t="s">
+      <c r="K25" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>39</v>
       </c>
@@ -15282,7 +15274,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="14" t="str">
-        <f>$F26&amp;"."&amp;$G26&amp;"."&amp;$H26</f>
+        <f t="shared" si="0"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K26" s="14" t="s">
@@ -15319,14 +15311,14 @@
         <v>0</v>
       </c>
       <c r="J27" s="2" t="str">
-        <f>$F27&amp;"."&amp;$G27&amp;"."&amp;$H27</f>
+        <f t="shared" si="0"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
@@ -15356,14 +15348,14 @@
         <v>0</v>
       </c>
       <c r="J28" s="2" t="str">
-        <f>$F28&amp;"."&amp;$G28&amp;"."&amp;$H28</f>
+        <f t="shared" si="0"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>35</v>
       </c>
@@ -15393,7 +15385,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="2" t="str">
-        <f>$F29&amp;"."&amp;$G29&amp;"."&amp;$H29</f>
+        <f t="shared" si="0"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K29" s="2" t="s">
@@ -15430,14 +15422,14 @@
         <v>0</v>
       </c>
       <c r="J30" s="2" t="str">
-        <f>$F30&amp;"."&amp;$G30&amp;"."&amp;$H30</f>
+        <f t="shared" si="0"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
@@ -15467,14 +15459,14 @@
         <v>4</v>
       </c>
       <c r="J31" s="2" t="str">
-        <f>$F31&amp;"."&amp;$G31&amp;"."&amp;$H31</f>
+        <f t="shared" si="0"/>
         <v>none.none.no</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -15504,14 +15496,14 @@
         <v>4</v>
       </c>
       <c r="J32" s="2" t="str">
-        <f>$F32&amp;"."&amp;$G32&amp;"."&amp;$H32</f>
+        <f t="shared" si="0"/>
         <v>none.none.no</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
@@ -15541,14 +15533,14 @@
         <v>4</v>
       </c>
       <c r="J33" s="2" t="str">
-        <f>$F33&amp;"."&amp;$G33&amp;"."&amp;$H33</f>
+        <f t="shared" si="0"/>
         <v>none.none.no</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>37</v>
       </c>
@@ -15578,14 +15570,14 @@
         <v>1</v>
       </c>
       <c r="J34" s="14" t="str">
-        <f>$F34&amp;"."&amp;$G34&amp;"."&amp;$H34</f>
+        <f t="shared" ref="J34:J65" si="1">$F34&amp;"."&amp;$G34&amp;"."&amp;$H34</f>
         <v>correct.none.yes</v>
       </c>
       <c r="K34" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -15615,7 +15607,7 @@
         <v>1</v>
       </c>
       <c r="J35" s="2" t="str">
-        <f>$F35&amp;"."&amp;$G35&amp;"."&amp;$H35</f>
+        <f t="shared" si="1"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K35" s="2" t="s">
@@ -15652,14 +15644,14 @@
         <v>1</v>
       </c>
       <c r="J36" s="2" t="str">
-        <f>$F36&amp;"."&amp;$G36&amp;"."&amp;$H36</f>
+        <f t="shared" si="1"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>38</v>
       </c>
@@ -15689,7 +15681,7 @@
         <v>1</v>
       </c>
       <c r="J37" s="2" t="str">
-        <f>$F37&amp;"."&amp;$G37&amp;"."&amp;$H37</f>
+        <f t="shared" si="1"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K37" s="2" t="s">
@@ -15726,14 +15718,14 @@
         <v>1</v>
       </c>
       <c r="J38" s="2" t="str">
-        <f>$F38&amp;"."&amp;$G38&amp;"."&amp;$H38</f>
+        <f t="shared" si="1"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>33</v>
       </c>
@@ -15763,14 +15755,14 @@
         <v>4</v>
       </c>
       <c r="J39" s="2" t="str">
-        <f>$F39&amp;"."&amp;$G39&amp;"."&amp;$H39</f>
+        <f t="shared" si="1"/>
         <v>none.none.no</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>34</v>
       </c>
@@ -15800,14 +15792,14 @@
         <v>4</v>
       </c>
       <c r="J40" s="2" t="str">
-        <f>$F40&amp;"."&amp;$G40&amp;"."&amp;$H40</f>
+        <f t="shared" si="1"/>
         <v>none.none.no</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>35</v>
       </c>
@@ -15837,14 +15829,14 @@
         <v>4</v>
       </c>
       <c r="J41" s="2" t="str">
-        <f>$F41&amp;"."&amp;$G41&amp;"."&amp;$H41</f>
+        <f t="shared" si="1"/>
         <v>none.none.no</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>37</v>
       </c>
@@ -15874,14 +15866,14 @@
         <v>1</v>
       </c>
       <c r="J42" s="14" t="str">
-        <f>$F42&amp;"."&amp;$G42&amp;"."&amp;$H42</f>
+        <f t="shared" si="1"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K42" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>39</v>
       </c>
@@ -15911,7 +15903,7 @@
         <v>1</v>
       </c>
       <c r="J43" s="2" t="str">
-        <f>$F43&amp;"."&amp;$G43&amp;"."&amp;$H43</f>
+        <f t="shared" si="1"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K43" s="2" t="s">
@@ -15948,14 +15940,14 @@
         <v>1</v>
       </c>
       <c r="J44" s="2" t="str">
-        <f>$F44&amp;"."&amp;$G44&amp;"."&amp;$H44</f>
+        <f t="shared" si="1"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>38</v>
       </c>
@@ -15985,7 +15977,7 @@
         <v>1</v>
       </c>
       <c r="J45" s="2" t="str">
-        <f>$F45&amp;"."&amp;$G45&amp;"."&amp;$H45</f>
+        <f t="shared" si="1"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K45" s="2" t="s">
@@ -16022,14 +16014,14 @@
         <v>1</v>
       </c>
       <c r="J46" s="2" t="str">
-        <f>$F46&amp;"."&amp;$G46&amp;"."&amp;$H46</f>
+        <f t="shared" si="1"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>33</v>
       </c>
@@ -16059,21 +16051,21 @@
         <v>4</v>
       </c>
       <c r="J47" s="2" t="str">
-        <f>$F47&amp;"."&amp;$G47&amp;"."&amp;$H47</f>
+        <f t="shared" si="1"/>
         <v>none.none.no</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="65" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="65" t="s">
+      <c r="B48" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="65" t="s">
+      <c r="C48" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D48" s="57" t="s">
@@ -16082,28 +16074,28 @@
       <c r="E48" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="F48" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G48" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H48" s="65" t="s">
+      <c r="F48" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I48" s="65">
+      <c r="I48" s="2">
         <f>IFERROR(INT(IF($J48=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J48=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J48=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J48=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J48=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J48=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J48=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J48=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J48=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J48=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J48=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J48=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J48=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J48=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J48=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J48=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J48=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J48=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J48=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J48=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J48=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J48=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J48=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J48=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J48=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J48=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J48=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>4</v>
       </c>
-      <c r="J48" s="65" t="str">
-        <f>$F48&amp;"."&amp;$G48&amp;"."&amp;$H48</f>
+      <c r="J48" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>none.none.no</v>
       </c>
-      <c r="K48" s="65" t="s">
+      <c r="K48" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>35</v>
       </c>
@@ -16133,14 +16125,14 @@
         <v>4</v>
       </c>
       <c r="J49" s="2" t="str">
-        <f>$F49&amp;"."&amp;$G49&amp;"."&amp;$H49</f>
+        <f t="shared" si="1"/>
         <v>none.none.no</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
         <v>33</v>
       </c>
@@ -16170,14 +16162,14 @@
         <v>0</v>
       </c>
       <c r="J50" s="14" t="str">
-        <f>$F50&amp;"."&amp;$G50&amp;"."&amp;$H50</f>
+        <f t="shared" si="1"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K50" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>35</v>
       </c>
@@ -16207,14 +16199,14 @@
         <v>0</v>
       </c>
       <c r="J51" s="2" t="str">
-        <f>$F51&amp;"."&amp;$G51&amp;"."&amp;$H51</f>
+        <f t="shared" si="1"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K51" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>39</v>
       </c>
@@ -16244,7 +16236,7 @@
         <v>1</v>
       </c>
       <c r="J52" s="2" t="str">
-        <f>$F52&amp;"."&amp;$G52&amp;"."&amp;$H52</f>
+        <f t="shared" si="1"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K52" s="2" t="s">
@@ -16281,7 +16273,7 @@
         <v>1</v>
       </c>
       <c r="J53" s="2" t="str">
-        <f>$F53&amp;"."&amp;$G53&amp;"."&amp;$H53</f>
+        <f t="shared" si="1"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K53" s="2" t="s">
@@ -16318,14 +16310,14 @@
         <v>1</v>
       </c>
       <c r="J54" s="2" t="str">
-        <f>$F54&amp;"."&amp;$G54&amp;"."&amp;$H54</f>
+        <f t="shared" si="1"/>
         <v>correct.warning.no</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>37</v>
       </c>
@@ -16355,14 +16347,14 @@
         <v>4</v>
       </c>
       <c r="J55" s="2" t="str">
-        <f>$F55&amp;"."&amp;$G55&amp;"."&amp;$H55</f>
+        <f t="shared" si="1"/>
         <v>misleading.none.yes</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>38</v>
       </c>
@@ -16392,14 +16384,14 @@
         <v>4</v>
       </c>
       <c r="J56" s="2" t="str">
-        <f>$F56&amp;"."&amp;$G56&amp;"."&amp;$H56</f>
+        <f t="shared" si="1"/>
         <v>none.none.no</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>34</v>
       </c>
@@ -16429,14 +16421,14 @@
         <v>4</v>
       </c>
       <c r="J57" s="2" t="str">
-        <f>$F57&amp;"."&amp;$G57&amp;"."&amp;$H57</f>
+        <f t="shared" si="1"/>
         <v>none.none.no</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
         <v>37</v>
       </c>
@@ -16466,7 +16458,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="14" t="str">
-        <f>$F58&amp;"."&amp;$G58&amp;"."&amp;$H58</f>
+        <f t="shared" si="1"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K58" s="14" t="s">
@@ -16474,13 +16466,13 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" s="65" t="s">
+      <c r="A59" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B59" s="65" t="s">
+      <c r="B59" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C59" s="65" t="s">
+      <c r="C59" s="2" t="s">
         <v>186</v>
       </c>
       <c r="D59" s="58" t="s">
@@ -16489,24 +16481,24 @@
       <c r="E59" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="F59" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G59" s="65" t="s">
+      <c r="F59" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G59" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="65" t="s">
+      <c r="H59" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I59" s="65">
+      <c r="I59" s="2">
         <f>IFERROR(INT(IF($J59=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J59=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J59=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J59=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J59=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J59=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J59=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J59=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J59=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J59=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J59=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J59=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J59=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J59=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J59=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J59=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J59=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J59=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J59=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J59=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J59=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J59=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J59=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J59=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J59=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J59=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J59=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>0</v>
       </c>
-      <c r="J59" s="65" t="str">
-        <f>$F59&amp;"."&amp;$G59&amp;"."&amp;$H59</f>
+      <c r="J59" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>none.blocked.no</v>
       </c>
-      <c r="K59" s="65" t="s">
+      <c r="K59" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -16540,14 +16532,14 @@
         <v>0</v>
       </c>
       <c r="J60" s="2" t="str">
-        <f>$F60&amp;"."&amp;$G60&amp;"."&amp;$H60</f>
+        <f t="shared" si="1"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>39</v>
       </c>
@@ -16577,14 +16569,14 @@
         <v>4</v>
       </c>
       <c r="J61" s="2" t="str">
-        <f>$F61&amp;"."&amp;$G61&amp;"."&amp;$H61</f>
+        <f t="shared" si="1"/>
         <v>none.none.no</v>
       </c>
       <c r="K61" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>38</v>
       </c>
@@ -16614,14 +16606,14 @@
         <v>4</v>
       </c>
       <c r="J62" s="2" t="str">
-        <f>$F62&amp;"."&amp;$G62&amp;"."&amp;$H62</f>
+        <f t="shared" si="1"/>
         <v>none.none.no</v>
       </c>
       <c r="K62" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>33</v>
       </c>
@@ -16651,21 +16643,21 @@
         <v>4</v>
       </c>
       <c r="J63" s="2" t="str">
-        <f>$F63&amp;"."&amp;$G63&amp;"."&amp;$H63</f>
+        <f t="shared" si="1"/>
         <v>none.none.no</v>
       </c>
       <c r="K63" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="65" t="s">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="65" t="s">
+      <c r="B64" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C64" s="65" t="s">
+      <c r="C64" s="2" t="s">
         <v>186</v>
       </c>
       <c r="D64" s="58" t="s">
@@ -16674,28 +16666,28 @@
       <c r="E64" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="F64" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G64" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H64" s="65" t="s">
+      <c r="F64" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H64" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I64" s="65">
+      <c r="I64" s="2">
         <f>IFERROR(INT(IF($J64=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J64=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J64=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J64=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J64=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J64=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J64=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J64=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J64=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J64=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J64=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J64=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J64=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J64=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J64=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J64=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J64=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J64=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J64=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J64=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J64=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J64=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J64=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J64=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J64=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J64=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J64=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>4</v>
       </c>
-      <c r="J64" s="65" t="str">
-        <f>$F64&amp;"."&amp;$G64&amp;"."&amp;$H64</f>
+      <c r="J64" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>none.none.no</v>
       </c>
-      <c r="K64" s="65" t="s">
+      <c r="K64" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>35</v>
       </c>
@@ -16725,14 +16717,14 @@
         <v>4</v>
       </c>
       <c r="J65" s="2" t="str">
-        <f>$F65&amp;"."&amp;$G65&amp;"."&amp;$H65</f>
+        <f t="shared" si="1"/>
         <v>none.none.no</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
         <v>37</v>
       </c>
@@ -16762,14 +16754,14 @@
         <v>0</v>
       </c>
       <c r="J66" s="14" t="str">
-        <f>$F66&amp;"."&amp;$G66&amp;"."&amp;$H66</f>
+        <f t="shared" ref="J66:J97" si="2">$F66&amp;"."&amp;$G66&amp;"."&amp;$H66</f>
         <v>none.blocked.no</v>
       </c>
       <c r="K66" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>39</v>
       </c>
@@ -16799,7 +16791,7 @@
         <v>0</v>
       </c>
       <c r="J67" s="2" t="str">
-        <f>$F67&amp;"."&amp;$G67&amp;"."&amp;$H67</f>
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K67" s="2" t="s">
@@ -16836,14 +16828,14 @@
         <v>0</v>
       </c>
       <c r="J68" s="2" t="str">
-        <f>$F68&amp;"."&amp;$G68&amp;"."&amp;$H68</f>
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K68" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>38</v>
       </c>
@@ -16873,14 +16865,14 @@
         <v>0</v>
       </c>
       <c r="J69" s="2" t="str">
-        <f>$F69&amp;"."&amp;$G69&amp;"."&amp;$H69</f>
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K69" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>33</v>
       </c>
@@ -16910,14 +16902,14 @@
         <v>0</v>
       </c>
       <c r="J70" s="2" t="str">
-        <f>$F70&amp;"."&amp;$G70&amp;"."&amp;$H70</f>
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K70" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>34</v>
       </c>
@@ -16947,21 +16939,21 @@
         <v>0</v>
       </c>
       <c r="J71" s="2" t="str">
-        <f>$F71&amp;"."&amp;$G71&amp;"."&amp;$H71</f>
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K71" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="65" t="s">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B72" s="65" t="s">
+      <c r="B72" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C72" s="65" t="s">
+      <c r="C72" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D72" s="58" t="s">
@@ -16970,35 +16962,35 @@
       <c r="E72" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="F72" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G72" s="65" t="s">
+      <c r="F72" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G72" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H72" s="65" t="s">
+      <c r="H72" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I72" s="65">
+      <c r="I72" s="2">
         <f>IFERROR(INT(IF($J72=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J72=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J72=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J72=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J72=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J72=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J72=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J72=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J72=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J72=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J72=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J72=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J72=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J72=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J72=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J72=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J72=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J72=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J72=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J72=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J72=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J72=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J72=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J72=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J72=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J72=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J72=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>0</v>
       </c>
-      <c r="J72" s="65" t="str">
-        <f>$F72&amp;"."&amp;$G72&amp;"."&amp;$H72</f>
+      <c r="J72" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
-      <c r="K72" s="65" t="s">
+      <c r="K72" s="2" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" s="65" t="s">
+      <c r="A73" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B73" s="65" t="s">
+      <c r="B73" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C73" s="65" t="s">
+      <c r="C73" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D73" s="58" t="s">
@@ -17007,28 +16999,28 @@
       <c r="E73" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="F73" s="65" t="s">
+      <c r="F73" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G73" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H73" s="65" t="s">
+      <c r="G73" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H73" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I73" s="65">
+      <c r="I73" s="2">
         <f>IFERROR(INT(IF($J73=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J73=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J73=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J73=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J73=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J73=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J73=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J73=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J73=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J73=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J73=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J73=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J73=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J73=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J73=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J73=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J73=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J73=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J73=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J73=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J73=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J73=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J73=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J73=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J73=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J73=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J73=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>1</v>
       </c>
-      <c r="J73" s="65" t="str">
-        <f>$F73&amp;"."&amp;$G73&amp;"."&amp;$H73</f>
+      <c r="J73" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
-      <c r="K73" s="65" t="s">
+      <c r="K73" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="14" t="s">
         <v>37</v>
       </c>
@@ -17058,14 +17050,14 @@
         <v>0</v>
       </c>
       <c r="J74" s="14" t="str">
-        <f>$F74&amp;"."&amp;$G74&amp;"."&amp;$H74</f>
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K74" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>39</v>
       </c>
@@ -17095,7 +17087,7 @@
         <v>0</v>
       </c>
       <c r="J75" s="2" t="str">
-        <f>$F75&amp;"."&amp;$G75&amp;"."&amp;$H75</f>
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K75" s="2" t="s">
@@ -17132,14 +17124,14 @@
         <v>0</v>
       </c>
       <c r="J76" s="2" t="str">
-        <f>$F76&amp;"."&amp;$G76&amp;"."&amp;$H76</f>
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K76" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>38</v>
       </c>
@@ -17169,14 +17161,14 @@
         <v>0</v>
       </c>
       <c r="J77" s="2" t="str">
-        <f>$F77&amp;"."&amp;$G77&amp;"."&amp;$H77</f>
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K77" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>33</v>
       </c>
@@ -17206,14 +17198,14 @@
         <v>0</v>
       </c>
       <c r="J78" s="2" t="str">
-        <f>$F78&amp;"."&amp;$G78&amp;"."&amp;$H78</f>
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K78" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>34</v>
       </c>
@@ -17243,14 +17235,14 @@
         <v>0</v>
       </c>
       <c r="J79" s="2" t="str">
-        <f>$F79&amp;"."&amp;$G79&amp;"."&amp;$H79</f>
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K79" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>35</v>
       </c>
@@ -17280,7 +17272,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="2" t="str">
-        <f>$F80&amp;"."&amp;$G80&amp;"."&amp;$H80</f>
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K80" s="2" t="s">
@@ -17317,14 +17309,14 @@
         <v>1</v>
       </c>
       <c r="J81" s="2" t="str">
-        <f>$F81&amp;"."&amp;$G81&amp;"."&amp;$H81</f>
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K81" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="82" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="14" t="s">
         <v>34</v>
       </c>
@@ -17354,14 +17346,14 @@
         <v>0</v>
       </c>
       <c r="J82" s="14" t="str">
-        <f>$F82&amp;"."&amp;$G82&amp;"."&amp;$H82</f>
+        <f t="shared" si="2"/>
         <v>correct.blocked.yes</v>
       </c>
       <c r="K82" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>37</v>
       </c>
@@ -17391,14 +17383,14 @@
         <v>1</v>
       </c>
       <c r="J83" s="2" t="str">
-        <f>$F83&amp;"."&amp;$G83&amp;"."&amp;$H83</f>
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K83" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>39</v>
       </c>
@@ -17428,7 +17420,7 @@
         <v>1</v>
       </c>
       <c r="J84" s="2" t="str">
-        <f>$F84&amp;"."&amp;$G84&amp;"."&amp;$H84</f>
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K84" s="2" t="s">
@@ -17465,14 +17457,14 @@
         <v>1</v>
       </c>
       <c r="J85" s="2" t="str">
-        <f>$F85&amp;"."&amp;$G85&amp;"."&amp;$H85</f>
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K85" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>38</v>
       </c>
@@ -17502,14 +17494,14 @@
         <v>1</v>
       </c>
       <c r="J86" s="2" t="str">
-        <f>$F86&amp;"."&amp;$G86&amp;"."&amp;$H86</f>
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K86" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>33</v>
       </c>
@@ -17539,14 +17531,14 @@
         <v>1</v>
       </c>
       <c r="J87" s="2" t="str">
-        <f>$F87&amp;"."&amp;$G87&amp;"."&amp;$H87</f>
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K87" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>35</v>
       </c>
@@ -17576,7 +17568,7 @@
         <v>1</v>
       </c>
       <c r="J88" s="2" t="str">
-        <f>$F88&amp;"."&amp;$G88&amp;"."&amp;$H88</f>
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K88" s="2" t="s">
@@ -17584,13 +17576,13 @@
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A89" s="65" t="s">
+      <c r="A89" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B89" s="65" t="s">
+      <c r="B89" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C89" s="65" t="s">
+      <c r="C89" s="2" t="s">
         <v>185</v>
       </c>
       <c r="D89" s="58" t="s">
@@ -17599,24 +17591,24 @@
       <c r="E89" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="F89" s="65" t="s">
+      <c r="F89" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G89" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H89" s="65" t="s">
+      <c r="G89" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H89" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I89" s="65">
+      <c r="I89" s="2">
         <f>IFERROR(INT(IF($J89=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J89=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J89=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J89=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J89=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J89=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J89=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J89=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J89=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J89=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J89=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J89=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J89=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J89=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J89=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J89=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J89=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J89=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J89=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J89=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J89=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J89=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J89=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J89=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J89=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J89=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J89=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>1</v>
       </c>
-      <c r="J89" s="65" t="str">
-        <f>$F89&amp;"."&amp;$G89&amp;"."&amp;$H89</f>
+      <c r="J89" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
-      <c r="K89" s="65" t="s">
+      <c r="K89" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -17650,14 +17642,14 @@
         <v>0</v>
       </c>
       <c r="J90" s="14" t="str">
-        <f>$F90&amp;"."&amp;$G90&amp;"."&amp;$H90</f>
+        <f t="shared" si="2"/>
         <v>none.blocked.no</v>
       </c>
       <c r="K90" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>37</v>
       </c>
@@ -17687,14 +17679,14 @@
         <v>1</v>
       </c>
       <c r="J91" s="2" t="str">
-        <f>$F91&amp;"."&amp;$G91&amp;"."&amp;$H91</f>
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K91" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>39</v>
       </c>
@@ -17724,14 +17716,14 @@
         <v>1</v>
       </c>
       <c r="J92" s="2" t="str">
-        <f>$F92&amp;"."&amp;$G92&amp;"."&amp;$H92</f>
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K92" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>38</v>
       </c>
@@ -17761,14 +17753,14 @@
         <v>1</v>
       </c>
       <c r="J93" s="2" t="str">
-        <f>$F93&amp;"."&amp;$G93&amp;"."&amp;$H93</f>
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K93" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>33</v>
       </c>
@@ -17798,14 +17790,14 @@
         <v>1</v>
       </c>
       <c r="J94" s="2" t="str">
-        <f>$F94&amp;"."&amp;$G94&amp;"."&amp;$H94</f>
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K94" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>34</v>
       </c>
@@ -17825,24 +17817,24 @@
         <v>20</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I95" s="2">
         <f>IFERROR(INT(IF($J95=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J95=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J95=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J95=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J95=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J95=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J95=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J95=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J95=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J95=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J95=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J95=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J95=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J95=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J95=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J95=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J95=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J95=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J95=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J95=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J95=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J95=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J95=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J95=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J95=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J95=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J95=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J95" s="2" t="str">
-        <f>$F95&amp;"."&amp;$G95&amp;"."&amp;$H95</f>
-        <v>correct.none.yes</v>
+        <f t="shared" si="2"/>
+        <v>correct.blocked.yes</v>
       </c>
       <c r="K95" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>35</v>
       </c>
@@ -17862,18 +17854,18 @@
         <v>20</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H96" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I96" s="2">
         <f>IFERROR(INT(IF($J96=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J96=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J96=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J96=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J96=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J96=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J96=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J96=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J96=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J96=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J96=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J96=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J96=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J96=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J96=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J96=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J96=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J96=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J96=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J96=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J96=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J96=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J96=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J96=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J96=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J96=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J96=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J96" s="2" t="str">
-        <f>$F96&amp;"."&amp;$G96&amp;"."&amp;$H96</f>
-        <v>correct.blocked.yes</v>
+        <f t="shared" si="2"/>
+        <v>correct.none.yes</v>
       </c>
       <c r="K96" s="2" t="s">
         <v>180</v>
@@ -17909,14 +17901,14 @@
         <v>1</v>
       </c>
       <c r="J97" s="2" t="str">
-        <f>$F97&amp;"."&amp;$G97&amp;"."&amp;$H97</f>
+        <f t="shared" si="2"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K97" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="98" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="14" t="s">
         <v>37</v>
       </c>
@@ -17946,14 +17938,14 @@
         <v>4</v>
       </c>
       <c r="J98" s="14" t="str">
-        <f>$F98&amp;"."&amp;$G98&amp;"."&amp;$H98</f>
+        <f t="shared" ref="J98:J129" si="3">$F98&amp;"."&amp;$G98&amp;"."&amp;$H98</f>
         <v>misleading.none.no</v>
       </c>
       <c r="K98" s="14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>39</v>
       </c>
@@ -17983,7 +17975,7 @@
         <v>4</v>
       </c>
       <c r="J99" s="2" t="str">
-        <f>$F99&amp;"."&amp;$G99&amp;"."&amp;$H99</f>
+        <f t="shared" si="3"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K99" s="2" t="s">
@@ -18020,14 +18012,14 @@
         <v>4</v>
       </c>
       <c r="J100" s="2" t="str">
-        <f>$F100&amp;"."&amp;$G100&amp;"."&amp;$H100</f>
+        <f t="shared" si="3"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K100" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>38</v>
       </c>
@@ -18057,14 +18049,14 @@
         <v>4</v>
       </c>
       <c r="J101" s="2" t="str">
-        <f>$F101&amp;"."&amp;$G101&amp;"."&amp;$H101</f>
+        <f t="shared" si="3"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K101" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>33</v>
       </c>
@@ -18094,14 +18086,14 @@
         <v>4</v>
       </c>
       <c r="J102" s="2" t="str">
-        <f>$F102&amp;"."&amp;$G102&amp;"."&amp;$H102</f>
+        <f t="shared" si="3"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K102" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>34</v>
       </c>
@@ -18131,21 +18123,21 @@
         <v>4</v>
       </c>
       <c r="J103" s="2" t="str">
-        <f>$F103&amp;"."&amp;$G103&amp;"."&amp;$H103</f>
+        <f t="shared" si="3"/>
         <v>misleading.none.yes</v>
       </c>
       <c r="K103" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="65" t="s">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B104" s="65" t="s">
+      <c r="B104" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C104" s="65" t="s">
+      <c r="C104" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D104" s="57" t="s">
@@ -18154,24 +18146,24 @@
       <c r="E104" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="F104" s="65" t="s">
+      <c r="F104" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G104" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H104" s="65" t="s">
+      <c r="G104" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H104" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I104" s="65">
+      <c r="I104" s="2">
         <f>IFERROR(INT(IF($J104=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J104=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J104=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J104=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J104=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J104=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J104=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J104=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J104=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J104=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J104=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J104=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J104=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J104=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J104=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J104=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J104=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J104=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J104=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J104=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J104=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J104=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J104=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J104=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J104=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J104=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J104=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>4</v>
       </c>
-      <c r="J104" s="65" t="str">
-        <f>$F104&amp;"."&amp;$G104&amp;"."&amp;$H104</f>
+      <c r="J104" s="2" t="str">
+        <f t="shared" si="3"/>
         <v>misleading.none.no</v>
       </c>
-      <c r="K104" s="65" t="s">
+      <c r="K104" s="2" t="s">
         <v>179</v>
       </c>
     </row>
@@ -18205,7 +18197,7 @@
         <v>4</v>
       </c>
       <c r="J105" s="2" t="str">
-        <f>$F105&amp;"."&amp;$G105&amp;"."&amp;$H105</f>
+        <f t="shared" si="3"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K105" s="2" t="s">
@@ -18242,14 +18234,14 @@
         <v>1</v>
       </c>
       <c r="J106" s="14" t="str">
-        <f>$F106&amp;"."&amp;$G106&amp;"."&amp;$H106</f>
+        <f t="shared" si="3"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K106" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>37</v>
       </c>
@@ -18279,14 +18271,14 @@
         <v>4</v>
       </c>
       <c r="J107" s="2" t="str">
-        <f>$F107&amp;"."&amp;$G107&amp;"."&amp;$H107</f>
+        <f t="shared" si="3"/>
         <v>misleading.none.yes</v>
       </c>
       <c r="K107" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>39</v>
       </c>
@@ -18316,7 +18308,7 @@
         <v>4</v>
       </c>
       <c r="J108" s="2" t="str">
-        <f>$F108&amp;"."&amp;$G108&amp;"."&amp;$H108</f>
+        <f t="shared" si="3"/>
         <v>misleading.none.yes</v>
       </c>
       <c r="K108" s="2" t="s">
@@ -18353,14 +18345,14 @@
         <v>4</v>
       </c>
       <c r="J109" s="2" t="str">
-        <f>$F109&amp;"."&amp;$G109&amp;"."&amp;$H109</f>
+        <f t="shared" si="3"/>
         <v>misleading.none.yes</v>
       </c>
       <c r="K109" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>38</v>
       </c>
@@ -18390,14 +18382,14 @@
         <v>4</v>
       </c>
       <c r="J110" s="2" t="str">
-        <f>$F110&amp;"."&amp;$G110&amp;"."&amp;$H110</f>
+        <f t="shared" si="3"/>
         <v>misleading.none.yes</v>
       </c>
       <c r="K110" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>33</v>
       </c>
@@ -18427,14 +18419,14 @@
         <v>4</v>
       </c>
       <c r="J111" s="2" t="str">
-        <f>$F111&amp;"."&amp;$G111&amp;"."&amp;$H111</f>
+        <f t="shared" si="3"/>
         <v>none.none.no</v>
       </c>
       <c r="K111" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>34</v>
       </c>
@@ -18464,21 +18456,21 @@
         <v>4</v>
       </c>
       <c r="J112" s="2" t="str">
-        <f>$F112&amp;"."&amp;$G112&amp;"."&amp;$H112</f>
+        <f t="shared" si="3"/>
         <v>none.none.no</v>
       </c>
       <c r="K112" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="65" t="s">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B113" s="65" t="s">
+      <c r="B113" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C113" s="65" t="s">
+      <c r="C113" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D113" s="57" t="s">
@@ -18487,28 +18479,28 @@
       <c r="E113" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="F113" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G113" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H113" s="65" t="s">
+      <c r="F113" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H113" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I113" s="65">
+      <c r="I113" s="2">
         <f>IFERROR(INT(IF($J113=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J113=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J113=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J113=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J113=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J113=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J113=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J113=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J113=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J113=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J113=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J113=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J113=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J113=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J113=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J113=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J113=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J113=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J113=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J113=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J113=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J113=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J113=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J113=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J113=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J113=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J113=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>4</v>
       </c>
-      <c r="J113" s="65" t="str">
-        <f>$F113&amp;"."&amp;$G113&amp;"."&amp;$H113</f>
+      <c r="J113" s="2" t="str">
+        <f t="shared" si="3"/>
         <v>none.none.no</v>
       </c>
-      <c r="K113" s="65" t="s">
+      <c r="K113" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="114" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="14" t="s">
         <v>37</v>
       </c>
@@ -18538,7 +18530,7 @@
         <v>1</v>
       </c>
       <c r="J114" s="14" t="str">
-        <f>$F114&amp;"."&amp;$G114&amp;"."&amp;$H114</f>
+        <f t="shared" si="3"/>
         <v>correct.none.no</v>
       </c>
       <c r="K114" s="14" t="s">
@@ -18575,14 +18567,14 @@
         <v>1</v>
       </c>
       <c r="J115" s="2" t="str">
-        <f>$F115&amp;"."&amp;$G115&amp;"."&amp;$H115</f>
+        <f t="shared" si="3"/>
         <v>correct.none.no</v>
       </c>
       <c r="K115" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>38</v>
       </c>
@@ -18612,7 +18604,7 @@
         <v>1</v>
       </c>
       <c r="J116" s="2" t="str">
-        <f>$F116&amp;"."&amp;$G116&amp;"."&amp;$H116</f>
+        <f t="shared" si="3"/>
         <v>correct.none.no</v>
       </c>
       <c r="K116" s="2" t="s">
@@ -18649,14 +18641,14 @@
         <v>1</v>
       </c>
       <c r="J117" s="2" t="str">
-        <f>$F117&amp;"."&amp;$G117&amp;"."&amp;$H117</f>
+        <f t="shared" si="3"/>
         <v>correct.none.no</v>
       </c>
       <c r="K117" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>39</v>
       </c>
@@ -18686,14 +18678,14 @@
         <v>2</v>
       </c>
       <c r="J118" s="2" t="str">
-        <f>$F118&amp;"."&amp;$G118&amp;"."&amp;$H118</f>
+        <f t="shared" si="3"/>
         <v>both.none.no</v>
       </c>
       <c r="K118" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>33</v>
       </c>
@@ -18723,14 +18715,14 @@
         <v>2</v>
       </c>
       <c r="J119" s="2" t="str">
-        <f>$F119&amp;"."&amp;$G119&amp;"."&amp;$H119</f>
+        <f t="shared" si="3"/>
         <v>both.none.no</v>
       </c>
       <c r="K119" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>34</v>
       </c>
@@ -18760,21 +18752,21 @@
         <v>2</v>
       </c>
       <c r="J120" s="2" t="str">
-        <f>$F120&amp;"."&amp;$G120&amp;"."&amp;$H120</f>
+        <f t="shared" si="3"/>
         <v>both.none.no</v>
       </c>
       <c r="K120" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="65" t="s">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B121" s="65" t="s">
+      <c r="B121" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C121" s="65" t="s">
+      <c r="C121" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D121" s="57" t="s">
@@ -18783,28 +18775,28 @@
       <c r="E121" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="F121" s="65" t="s">
+      <c r="F121" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G121" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H121" s="65" t="s">
+      <c r="G121" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H121" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I121" s="65">
+      <c r="I121" s="2">
         <f>IFERROR(INT(IF($J121=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J121=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J121=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J121=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J121=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J121=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J121=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J121=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J121=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J121=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J121=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J121=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J121=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J121=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J121=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J121=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J121=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J121=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J121=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J121=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J121=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J121=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J121=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J121=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J121=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J121=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J121=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>2</v>
       </c>
-      <c r="J121" s="65" t="str">
-        <f>$F121&amp;"."&amp;$G121&amp;"."&amp;$H121</f>
+      <c r="J121" s="2" t="str">
+        <f t="shared" si="3"/>
         <v>both.none.no</v>
       </c>
-      <c r="K121" s="65" t="s">
+      <c r="K121" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="122" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="14" t="s">
         <v>37</v>
       </c>
@@ -18834,7 +18826,7 @@
         <v>2</v>
       </c>
       <c r="J122" s="14" t="str">
-        <f>$F122&amp;"."&amp;$G122&amp;"."&amp;$H122</f>
+        <f t="shared" si="3"/>
         <v>both.none.yes_same</v>
       </c>
       <c r="K122" s="14" t="s">
@@ -18871,7 +18863,7 @@
         <v>2</v>
       </c>
       <c r="J123" s="2" t="str">
-        <f>$F123&amp;"."&amp;$G123&amp;"."&amp;$H123</f>
+        <f t="shared" si="3"/>
         <v>both.none.no</v>
       </c>
       <c r="K123" s="2" t="s">
@@ -18908,14 +18900,14 @@
         <v>2</v>
       </c>
       <c r="J124" s="2" t="str">
-        <f>$F124&amp;"."&amp;$G124&amp;"."&amp;$H124</f>
+        <f t="shared" si="3"/>
         <v>both.none.no</v>
       </c>
       <c r="K124" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>39</v>
       </c>
@@ -18945,14 +18937,14 @@
         <v>4</v>
       </c>
       <c r="J125" s="2" t="str">
-        <f>$F125&amp;"."&amp;$G125&amp;"."&amp;$H125</f>
+        <f t="shared" si="3"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K125" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>38</v>
       </c>
@@ -18982,14 +18974,14 @@
         <v>4</v>
       </c>
       <c r="J126" s="2" t="str">
-        <f>$F126&amp;"."&amp;$G126&amp;"."&amp;$H126</f>
+        <f t="shared" si="3"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K126" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>33</v>
       </c>
@@ -19019,14 +19011,14 @@
         <v>4</v>
       </c>
       <c r="J127" s="2" t="str">
-        <f>$F127&amp;"."&amp;$G127&amp;"."&amp;$H127</f>
+        <f t="shared" si="3"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K127" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>34</v>
       </c>
@@ -19056,14 +19048,14 @@
         <v>4</v>
       </c>
       <c r="J128" s="2" t="str">
-        <f>$F128&amp;"."&amp;$G128&amp;"."&amp;$H128</f>
+        <f t="shared" si="3"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K128" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>35</v>
       </c>
@@ -19093,14 +19085,14 @@
         <v>4</v>
       </c>
       <c r="J129" s="2" t="str">
-        <f>$F129&amp;"."&amp;$G129&amp;"."&amp;$H129</f>
+        <f t="shared" si="3"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K129" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="14" t="s">
         <v>33</v>
       </c>
@@ -19130,14 +19122,14 @@
         <v>1</v>
       </c>
       <c r="J130" s="14" t="str">
-        <f>$F130&amp;"."&amp;$G130&amp;"."&amp;$H130</f>
+        <f t="shared" ref="J130:J161" si="4">$F130&amp;"."&amp;$G130&amp;"."&amp;$H130</f>
         <v>correct.none.no</v>
       </c>
       <c r="K130" s="14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>37</v>
       </c>
@@ -19167,14 +19159,14 @@
         <v>2</v>
       </c>
       <c r="J131" s="2" t="str">
-        <f>$F131&amp;"."&amp;$G131&amp;"."&amp;$H131</f>
+        <f t="shared" si="4"/>
         <v>both.none.yes_same</v>
       </c>
       <c r="K131" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>39</v>
       </c>
@@ -19204,7 +19196,7 @@
         <v>2</v>
       </c>
       <c r="J132" s="2" t="str">
-        <f>$F132&amp;"."&amp;$G132&amp;"."&amp;$H132</f>
+        <f t="shared" si="4"/>
         <v>both.none.yes_same</v>
       </c>
       <c r="K132" s="2" t="s">
@@ -19241,14 +19233,14 @@
         <v>2</v>
       </c>
       <c r="J133" s="2" t="str">
-        <f>$F133&amp;"."&amp;$G133&amp;"."&amp;$H133</f>
+        <f t="shared" si="4"/>
         <v>both.none.no</v>
       </c>
       <c r="K133" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>35</v>
       </c>
@@ -19278,7 +19270,7 @@
         <v>2</v>
       </c>
       <c r="J134" s="2" t="str">
-        <f>$F134&amp;"."&amp;$G134&amp;"."&amp;$H134</f>
+        <f t="shared" si="4"/>
         <v>both.none.yes_same</v>
       </c>
       <c r="K134" s="2" t="s">
@@ -19286,13 +19278,13 @@
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A135" s="65" t="s">
+      <c r="A135" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B135" s="65" t="s">
+      <c r="B135" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C135" s="65" t="s">
+      <c r="C135" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D135" s="58" t="s">
@@ -19301,28 +19293,28 @@
       <c r="E135" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="F135" s="65" t="s">
+      <c r="F135" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G135" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H135" s="65" t="s">
+      <c r="G135" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H135" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I135" s="65">
+      <c r="I135" s="2">
         <f>IFERROR(INT(IF($J135=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J135=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J135=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J135=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J135=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J135=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J135=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J135=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J135=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J135=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J135=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J135=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J135=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J135=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J135=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J135=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J135=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J135=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J135=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J135=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J135=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J135=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J135=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J135=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J135=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J135=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J135=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>2</v>
       </c>
-      <c r="J135" s="65" t="str">
-        <f>$F135&amp;"."&amp;$G135&amp;"."&amp;$H135</f>
+      <c r="J135" s="2" t="str">
+        <f t="shared" si="4"/>
         <v>both.none.no</v>
       </c>
-      <c r="K135" s="65" t="s">
+      <c r="K135" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>38</v>
       </c>
@@ -19352,14 +19344,14 @@
         <v>4</v>
       </c>
       <c r="J136" s="2" t="str">
-        <f>$F136&amp;"."&amp;$G136&amp;"."&amp;$H136</f>
+        <f t="shared" si="4"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K136" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>34</v>
       </c>
@@ -19389,14 +19381,14 @@
         <v>4</v>
       </c>
       <c r="J137" s="2" t="str">
-        <f>$F137&amp;"."&amp;$G137&amp;"."&amp;$H137</f>
+        <f t="shared" si="4"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K137" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="138" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="14" t="s">
         <v>37</v>
       </c>
@@ -19426,7 +19418,7 @@
         <v>2</v>
       </c>
       <c r="J138" s="14" t="str">
-        <f>$F138&amp;"."&amp;$G138&amp;"."&amp;$H138</f>
+        <f t="shared" si="4"/>
         <v>both.none.yes_same</v>
       </c>
       <c r="K138" s="14" t="s">
@@ -19463,7 +19455,7 @@
         <v>2</v>
       </c>
       <c r="J139" s="2" t="str">
-        <f>$F139&amp;"."&amp;$G139&amp;"."&amp;$H139</f>
+        <f t="shared" si="4"/>
         <v>both.none.no</v>
       </c>
       <c r="K139" s="2" t="s">
@@ -19500,21 +19492,21 @@
         <v>2</v>
       </c>
       <c r="J140" s="2" t="str">
-        <f>$F140&amp;"."&amp;$G140&amp;"."&amp;$H140</f>
+        <f t="shared" si="4"/>
         <v>both.none.no</v>
       </c>
       <c r="K140" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="65" t="s">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B141" s="65" t="s">
+      <c r="B141" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C141" s="65" t="s">
+      <c r="C141" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D141" s="57" t="s">
@@ -19523,28 +19515,28 @@
       <c r="E141" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="F141" s="65" t="s">
+      <c r="F141" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G141" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H141" s="65" t="s">
+      <c r="G141" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H141" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I141" s="65">
+      <c r="I141" s="2">
         <f>IFERROR(INT(IF($J141=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J141=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J141=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J141=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J141=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J141=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J141=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J141=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J141=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J141=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J141=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J141=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J141=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J141=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J141=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J141=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J141=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J141=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J141=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J141=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J141=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J141=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J141=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J141=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J141=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J141=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J141=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>4</v>
       </c>
-      <c r="J141" s="65" t="str">
-        <f>$F141&amp;"."&amp;$G141&amp;"."&amp;$H141</f>
+      <c r="J141" s="2" t="str">
+        <f t="shared" si="4"/>
         <v>both.none.yes_misleading-first</v>
       </c>
-      <c r="K141" s="65" t="s">
+      <c r="K141" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>38</v>
       </c>
@@ -19574,14 +19566,14 @@
         <v>4</v>
       </c>
       <c r="J142" s="2" t="str">
-        <f>$F142&amp;"."&amp;$G142&amp;"."&amp;$H142</f>
+        <f t="shared" si="4"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K142" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="143" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>33</v>
       </c>
@@ -19611,14 +19603,14 @@
         <v>4</v>
       </c>
       <c r="J143" s="2" t="str">
-        <f>$F143&amp;"."&amp;$G143&amp;"."&amp;$H143</f>
+        <f t="shared" si="4"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K143" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>34</v>
       </c>
@@ -19648,14 +19640,14 @@
         <v>4</v>
       </c>
       <c r="J144" s="2" t="str">
-        <f>$F144&amp;"."&amp;$G144&amp;"."&amp;$H144</f>
+        <f t="shared" si="4"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K144" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>35</v>
       </c>
@@ -19685,14 +19677,14 @@
         <v>4</v>
       </c>
       <c r="J145" s="2" t="str">
-        <f>$F145&amp;"."&amp;$G145&amp;"."&amp;$H145</f>
+        <f t="shared" si="4"/>
         <v>both.none.yes_misleading-first</v>
       </c>
       <c r="K145" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="146" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="14" t="s">
         <v>37</v>
       </c>
@@ -19722,14 +19714,14 @@
         <v>4</v>
       </c>
       <c r="J146" s="14" t="str">
-        <f>$F146&amp;"."&amp;$G146&amp;"."&amp;$H146</f>
+        <f t="shared" si="4"/>
         <v>misleading.none.yes</v>
       </c>
       <c r="K146" s="14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>39</v>
       </c>
@@ -19759,7 +19751,7 @@
         <v>4</v>
       </c>
       <c r="J147" s="2" t="str">
-        <f>$F147&amp;"."&amp;$G147&amp;"."&amp;$H147</f>
+        <f t="shared" si="4"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K147" s="2" t="s">
@@ -19796,21 +19788,21 @@
         <v>4</v>
       </c>
       <c r="J148" s="2" t="str">
-        <f>$F148&amp;"."&amp;$G148&amp;"."&amp;$H148</f>
+        <f t="shared" si="4"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K148" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="65" t="s">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B149" s="65" t="s">
+      <c r="B149" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C149" s="65" t="s">
+      <c r="C149" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D149" s="57" t="s">
@@ -19819,28 +19811,28 @@
       <c r="E149" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="F149" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G149" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H149" s="65" t="s">
+      <c r="F149" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G149" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H149" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I149" s="65">
+      <c r="I149" s="2">
         <f>IFERROR(INT(IF($J149=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J149=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J149=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J149=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J149=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J149=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J149=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J149=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J149=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J149=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J149=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J149=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J149=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J149=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J149=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J149=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J149=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J149=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J149=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J149=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J149=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J149=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J149=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J149=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J149=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J149=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J149=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>4</v>
       </c>
-      <c r="J149" s="65" t="str">
-        <f>$F149&amp;"."&amp;$G149&amp;"."&amp;$H149</f>
+      <c r="J149" s="2" t="str">
+        <f t="shared" si="4"/>
         <v>none.none.no</v>
       </c>
-      <c r="K149" s="65" t="s">
+      <c r="K149" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>33</v>
       </c>
@@ -19870,14 +19862,14 @@
         <v>4</v>
       </c>
       <c r="J150" s="2" t="str">
-        <f>$F150&amp;"."&amp;$G150&amp;"."&amp;$H150</f>
+        <f t="shared" si="4"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K150" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>34</v>
       </c>
@@ -19907,14 +19899,14 @@
         <v>4</v>
       </c>
       <c r="J151" s="2" t="str">
-        <f>$F151&amp;"."&amp;$G151&amp;"."&amp;$H151</f>
+        <f t="shared" si="4"/>
         <v>misleading.none.yes</v>
       </c>
       <c r="K151" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>35</v>
       </c>
@@ -19944,7 +19936,7 @@
         <v>4</v>
       </c>
       <c r="J152" s="2" t="str">
-        <f>$F152&amp;"."&amp;$G152&amp;"."&amp;$H152</f>
+        <f t="shared" si="4"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K152" s="2" t="s">
@@ -19981,14 +19973,14 @@
         <v>4</v>
       </c>
       <c r="J153" s="2" t="str">
-        <f>$F153&amp;"."&amp;$G153&amp;"."&amp;$H153</f>
+        <f t="shared" si="4"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K153" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="154" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="14" t="s">
         <v>37</v>
       </c>
@@ -20018,14 +20010,14 @@
         <v>1</v>
       </c>
       <c r="J154" s="14" t="str">
-        <f>$F154&amp;"."&amp;$G154&amp;"."&amp;$H154</f>
+        <f t="shared" si="4"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K154" s="14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>39</v>
       </c>
@@ -20055,7 +20047,7 @@
         <v>1</v>
       </c>
       <c r="J155" s="2" t="str">
-        <f>$F155&amp;"."&amp;$G155&amp;"."&amp;$H155</f>
+        <f t="shared" si="4"/>
         <v>correct.none.no</v>
       </c>
       <c r="K155" s="2" t="s">
@@ -20092,21 +20084,21 @@
         <v>1</v>
       </c>
       <c r="J156" s="2" t="str">
-        <f>$F156&amp;"."&amp;$G156&amp;"."&amp;$H156</f>
+        <f t="shared" si="4"/>
         <v>correct.none.no</v>
       </c>
       <c r="K156" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="65" t="s">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A157" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B157" s="65" t="s">
+      <c r="B157" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C157" s="65" t="s">
+      <c r="C157" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D157" s="57" t="s">
@@ -20115,28 +20107,28 @@
       <c r="E157" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="F157" s="65" t="s">
+      <c r="F157" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G157" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H157" s="65" t="s">
+      <c r="G157" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H157" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I157" s="65">
+      <c r="I157" s="2">
         <f>IFERROR(INT(IF($J157=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J157=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J157=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J157=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J157=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J157=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J157=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J157=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J157=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J157=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J157=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J157=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J157=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J157=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J157=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J157=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J157=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J157=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J157=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J157=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J157=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J157=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J157=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J157=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J157=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J157=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J157=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>1</v>
       </c>
-      <c r="J157" s="65" t="str">
-        <f>$F157&amp;"."&amp;$G157&amp;"."&amp;$H157</f>
+      <c r="J157" s="2" t="str">
+        <f t="shared" si="4"/>
         <v>correct.none.no</v>
       </c>
-      <c r="K157" s="65" t="s">
+      <c r="K157" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>33</v>
       </c>
@@ -20166,14 +20158,14 @@
         <v>1</v>
       </c>
       <c r="J158" s="2" t="str">
-        <f>$F158&amp;"."&amp;$G158&amp;"."&amp;$H158</f>
+        <f t="shared" si="4"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K158" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>34</v>
       </c>
@@ -20203,14 +20195,14 @@
         <v>1</v>
       </c>
       <c r="J159" s="2" t="str">
-        <f>$F159&amp;"."&amp;$G159&amp;"."&amp;$H159</f>
+        <f t="shared" si="4"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K159" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>35</v>
       </c>
@@ -20240,7 +20232,7 @@
         <v>1</v>
       </c>
       <c r="J160" s="2" t="str">
-        <f>$F160&amp;"."&amp;$G160&amp;"."&amp;$H160</f>
+        <f t="shared" si="4"/>
         <v>correct.none.no</v>
       </c>
       <c r="K160" s="2" t="s">
@@ -20277,14 +20269,14 @@
         <v>1</v>
       </c>
       <c r="J161" s="2" t="str">
-        <f>$F161&amp;"."&amp;$G161&amp;"."&amp;$H161</f>
+        <f t="shared" si="4"/>
         <v>correct.none.no</v>
       </c>
       <c r="K161" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="162" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="14" t="s">
         <v>37</v>
       </c>
@@ -20314,14 +20306,14 @@
         <v>1</v>
       </c>
       <c r="J162" s="14" t="str">
-        <f>$F162&amp;"."&amp;$G162&amp;"."&amp;$H162</f>
+        <f t="shared" ref="J162:J192" si="5">$F162&amp;"."&amp;$G162&amp;"."&amp;$H162</f>
         <v>correct.none.no</v>
       </c>
       <c r="K162" s="14" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>39</v>
       </c>
@@ -20351,7 +20343,7 @@
         <v>1</v>
       </c>
       <c r="J163" s="2" t="str">
-        <f>$F163&amp;"."&amp;$G163&amp;"."&amp;$H163</f>
+        <f t="shared" si="5"/>
         <v>correct.none.no</v>
       </c>
       <c r="K163" s="2" t="s">
@@ -20388,21 +20380,21 @@
         <v>1</v>
       </c>
       <c r="J164" s="2" t="str">
-        <f>$F164&amp;"."&amp;$G164&amp;"."&amp;$H164</f>
+        <f t="shared" si="5"/>
         <v>correct.none.no</v>
       </c>
       <c r="K164" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A165" s="65" t="s">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B165" s="65" t="s">
+      <c r="B165" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C165" s="65" t="s">
+      <c r="C165" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D165" s="57" t="s">
@@ -20411,28 +20403,28 @@
       <c r="E165" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="F165" s="65" t="s">
+      <c r="F165" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G165" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H165" s="65" t="s">
+      <c r="G165" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H165" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I165" s="65">
+      <c r="I165" s="2">
         <f>IFERROR(INT(IF($J165=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J165=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J165=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J165=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J165=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J165=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J165=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J165=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J165=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J165=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J165=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J165=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J165=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J165=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J165=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J165=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J165=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J165=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J165=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J165=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J165=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J165=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J165=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J165=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J165=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J165=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J165=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>1</v>
       </c>
-      <c r="J165" s="65" t="str">
-        <f>$F165&amp;"."&amp;$G165&amp;"."&amp;$H165</f>
+      <c r="J165" s="2" t="str">
+        <f t="shared" si="5"/>
         <v>correct.none.no</v>
       </c>
-      <c r="K165" s="65" t="s">
+      <c r="K165" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>34</v>
       </c>
@@ -20462,14 +20454,14 @@
         <v>1</v>
       </c>
       <c r="J166" s="2" t="str">
-        <f>$F166&amp;"."&amp;$G166&amp;"."&amp;$H166</f>
+        <f t="shared" si="5"/>
         <v>correct.none.no</v>
       </c>
       <c r="K166" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>35</v>
       </c>
@@ -20499,7 +20491,7 @@
         <v>1</v>
       </c>
       <c r="J167" s="2" t="str">
-        <f>$F167&amp;"."&amp;$G167&amp;"."&amp;$H167</f>
+        <f t="shared" si="5"/>
         <v>correct.none.no</v>
       </c>
       <c r="K167" s="2" t="s">
@@ -20536,14 +20528,14 @@
         <v>1</v>
       </c>
       <c r="J168" s="2" t="str">
-        <f>$F168&amp;"."&amp;$G168&amp;"."&amp;$H168</f>
+        <f t="shared" si="5"/>
         <v>correct.none.no</v>
       </c>
       <c r="K168" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>38</v>
       </c>
@@ -20573,14 +20565,14 @@
         <v>4</v>
       </c>
       <c r="J169" s="2" t="str">
-        <f>$F169&amp;"."&amp;$G169&amp;"."&amp;$H169</f>
+        <f t="shared" si="5"/>
         <v>none.none.no</v>
       </c>
       <c r="K169" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="170" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="14" t="s">
         <v>33</v>
       </c>
@@ -20610,14 +20602,14 @@
         <v>1</v>
       </c>
       <c r="J170" s="14" t="str">
-        <f>$F170&amp;"."&amp;$G170&amp;"."&amp;$H170</f>
+        <f t="shared" si="5"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K170" s="14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>37</v>
       </c>
@@ -20647,14 +20639,14 @@
         <v>4</v>
       </c>
       <c r="J171" s="2" t="str">
-        <f>$F171&amp;"."&amp;$G171&amp;"."&amp;$H171</f>
+        <f t="shared" si="5"/>
         <v>misleading.none.yes</v>
       </c>
       <c r="K171" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>39</v>
       </c>
@@ -20684,7 +20676,7 @@
         <v>4</v>
       </c>
       <c r="J172" s="2" t="str">
-        <f>$F172&amp;"."&amp;$G172&amp;"."&amp;$H172</f>
+        <f t="shared" si="5"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K172" s="2" t="s">
@@ -20692,13 +20684,13 @@
       </c>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A173" s="65" t="s">
+      <c r="A173" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B173" s="65" t="s">
+      <c r="B173" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C173" s="65" t="s">
+      <c r="C173" s="2" t="s">
         <v>181</v>
       </c>
       <c r="D173" s="57" t="s">
@@ -20707,28 +20699,28 @@
       <c r="E173" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="F173" s="65" t="s">
+      <c r="F173" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G173" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H173" s="65" t="s">
+      <c r="G173" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H173" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I173" s="65">
+      <c r="I173" s="2">
         <f>IFERROR(INT(IF($J173=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J173=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J173=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J173=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J173=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J173=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J173=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J173=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J173=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J173=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J173=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J173=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J173=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J173=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J173=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J173=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J173=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J173=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J173=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J173=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J173=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J173=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J173=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J173=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J173=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J173=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J173=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>4</v>
       </c>
-      <c r="J173" s="65" t="str">
-        <f>$F173&amp;"."&amp;$G173&amp;"."&amp;$H173</f>
+      <c r="J173" s="2" t="str">
+        <f t="shared" si="5"/>
         <v>misleading.none.no</v>
       </c>
-      <c r="K173" s="65" t="s">
+      <c r="K173" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>38</v>
       </c>
@@ -20758,14 +20750,14 @@
         <v>4</v>
       </c>
       <c r="J174" s="2" t="str">
-        <f>$F174&amp;"."&amp;$G174&amp;"."&amp;$H174</f>
+        <f t="shared" si="5"/>
         <v>none.none.no</v>
       </c>
       <c r="K174" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>34</v>
       </c>
@@ -20795,14 +20787,14 @@
         <v>4</v>
       </c>
       <c r="J175" s="2" t="str">
-        <f>$F175&amp;"."&amp;$G175&amp;"."&amp;$H175</f>
+        <f t="shared" si="5"/>
         <v>misleading.none.yes</v>
       </c>
       <c r="K175" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>35</v>
       </c>
@@ -20832,7 +20824,7 @@
         <v>4</v>
       </c>
       <c r="J176" s="2" t="str">
-        <f>$F176&amp;"."&amp;$G176&amp;"."&amp;$H176</f>
+        <f t="shared" si="5"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K176" s="2" t="s">
@@ -20869,14 +20861,14 @@
         <v>4</v>
       </c>
       <c r="J177" s="2" t="str">
-        <f>$F177&amp;"."&amp;$G177&amp;"."&amp;$H177</f>
+        <f t="shared" si="5"/>
         <v>misleading.none.no</v>
       </c>
       <c r="K177" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="178" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A178" s="14" t="s">
         <v>39</v>
       </c>
@@ -20906,7 +20898,7 @@
         <v>1</v>
       </c>
       <c r="J178" s="14" t="str">
-        <f>$F178&amp;"."&amp;$G178&amp;"."&amp;$H178</f>
+        <f t="shared" si="5"/>
         <v>correct.none.no</v>
       </c>
       <c r="K178" s="14" t="s">
@@ -20943,14 +20935,14 @@
         <v>1</v>
       </c>
       <c r="J179" s="2" t="str">
-        <f>$F179&amp;"."&amp;$G179&amp;"."&amp;$H179</f>
+        <f t="shared" si="5"/>
         <v>correct.none.no</v>
       </c>
       <c r="K179" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>38</v>
       </c>
@@ -20980,21 +20972,21 @@
         <v>1</v>
       </c>
       <c r="J180" s="2" t="str">
-        <f>$F180&amp;"."&amp;$G180&amp;"."&amp;$H180</f>
+        <f t="shared" si="5"/>
         <v>correct.none.no</v>
       </c>
       <c r="K180" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A181" s="65" t="s">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A181" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B181" s="65" t="s">
+      <c r="B181" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C181" s="65" t="s">
+      <c r="C181" s="2" t="s">
         <v>181</v>
       </c>
       <c r="D181" s="57" t="s">
@@ -21003,28 +20995,28 @@
       <c r="E181" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="F181" s="65" t="s">
+      <c r="F181" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G181" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H181" s="65" t="s">
+      <c r="G181" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H181" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I181" s="65">
+      <c r="I181" s="2">
         <f>IFERROR(INT(IF($J181=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J181=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J181=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J181=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J181=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J181=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J181=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J181=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J181=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J181=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J181=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J181=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J181=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J181=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J181=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J181=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J181=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J181=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J181=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J181=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J181=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J181=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J181=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J181=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J181=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J181=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J181=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>1</v>
       </c>
-      <c r="J181" s="65" t="str">
-        <f>$F181&amp;"."&amp;$G181&amp;"."&amp;$H181</f>
+      <c r="J181" s="2" t="str">
+        <f t="shared" si="5"/>
         <v>correct.none.yes</v>
       </c>
-      <c r="K181" s="65" t="s">
+      <c r="K181" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>35</v>
       </c>
@@ -21054,7 +21046,7 @@
         <v>1</v>
       </c>
       <c r="J182" s="2" t="str">
-        <f>$F182&amp;"."&amp;$G182&amp;"."&amp;$H182</f>
+        <f t="shared" si="5"/>
         <v>correct.none.no</v>
       </c>
       <c r="K182" s="2" t="s">
@@ -21091,14 +21083,14 @@
         <v>1</v>
       </c>
       <c r="J183" s="2" t="str">
-        <f>$F183&amp;"."&amp;$G183&amp;"."&amp;$H183</f>
+        <f t="shared" si="5"/>
         <v>correct.none.no</v>
       </c>
       <c r="K183" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>37</v>
       </c>
@@ -21128,14 +21120,14 @@
         <v>4</v>
       </c>
       <c r="J184" s="2" t="str">
-        <f>$F184&amp;"."&amp;$G184&amp;"."&amp;$H184</f>
+        <f t="shared" si="5"/>
         <v>misleading.none.yes</v>
       </c>
       <c r="K184" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>34</v>
       </c>
@@ -21165,14 +21157,14 @@
         <v>4</v>
       </c>
       <c r="J185" s="2" t="str">
-        <f>$F185&amp;"."&amp;$G185&amp;"."&amp;$H185</f>
+        <f t="shared" si="5"/>
         <v>misleading.none.yes</v>
       </c>
       <c r="K185" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="186" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A186" s="14" t="s">
         <v>37</v>
       </c>
@@ -21202,14 +21194,14 @@
         <v>1</v>
       </c>
       <c r="J186" s="14" t="str">
-        <f>$F186&amp;"."&amp;$G186&amp;"."&amp;$H186</f>
+        <f t="shared" si="5"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K186" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>39</v>
       </c>
@@ -21239,7 +21231,7 @@
         <v>1</v>
       </c>
       <c r="J187" s="2" t="str">
-        <f>$F187&amp;"."&amp;$G187&amp;"."&amp;$H187</f>
+        <f t="shared" si="5"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K187" s="2" t="s">
@@ -21276,7 +21268,7 @@
         <v>1</v>
       </c>
       <c r="J188" s="2" t="str">
-        <f>$F188&amp;"."&amp;$G188&amp;"."&amp;$H188</f>
+        <f t="shared" si="5"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K188" s="2" t="s">
@@ -21313,14 +21305,14 @@
         <v>1</v>
       </c>
       <c r="J189" s="2" t="str">
-        <f>$F189&amp;"."&amp;$G189&amp;"."&amp;$H189</f>
+        <f t="shared" si="5"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K189" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>33</v>
       </c>
@@ -21350,21 +21342,21 @@
         <v>4</v>
       </c>
       <c r="J190" s="2" t="str">
-        <f>$F190&amp;"."&amp;$G190&amp;"."&amp;$H190</f>
+        <f t="shared" si="5"/>
         <v>none.none.no</v>
       </c>
       <c r="K190" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="65" t="s">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A191" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B191" s="65" t="s">
+      <c r="B191" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C191" s="65" t="s">
+      <c r="C191" s="2" t="s">
         <v>181</v>
       </c>
       <c r="D191" s="57" t="s">
@@ -21373,28 +21365,28 @@
       <c r="E191" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="F191" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G191" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H191" s="65" t="s">
+      <c r="F191" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G191" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H191" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I191" s="65">
+      <c r="I191" s="2">
         <f>IFERROR(INT(IF($J191=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J191=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J191=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J191=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J191=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J191=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J191=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J191=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J191=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J191=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J191=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J191=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J191=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J191=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J191=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J191=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J191=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J191=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J191=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J191=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J191=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J191=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J191=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J191=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J191=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J191=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J191=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>4</v>
       </c>
-      <c r="J191" s="65" t="str">
-        <f>$F191&amp;"."&amp;$G191&amp;"."&amp;$H191</f>
+      <c r="J191" s="2" t="str">
+        <f t="shared" si="5"/>
         <v>none.none.no</v>
       </c>
-      <c r="K191" s="65" t="s">
+      <c r="K191" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>35</v>
       </c>
@@ -21424,14 +21416,14 @@
         <v>4</v>
       </c>
       <c r="J192" s="2" t="str">
-        <f>$F192&amp;"."&amp;$G192&amp;"."&amp;$H192</f>
+        <f t="shared" si="5"/>
         <v>none.none.no</v>
       </c>
       <c r="K192" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>38</v>
       </c>
@@ -21468,7 +21460,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="194" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194" s="14" t="s">
         <v>37</v>
       </c>
@@ -21498,14 +21490,14 @@
         <v>1</v>
       </c>
       <c r="J194" s="14" t="str">
-        <f>$F194&amp;"."&amp;$G194&amp;"."&amp;$H194</f>
+        <f t="shared" ref="J194:J208" si="6">$F194&amp;"."&amp;$G194&amp;"."&amp;$H194</f>
         <v>correct.none.yes</v>
       </c>
       <c r="K194" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>39</v>
       </c>
@@ -21535,7 +21527,7 @@
         <v>1</v>
       </c>
       <c r="J195" s="2" t="str">
-        <f>$F195&amp;"."&amp;$G195&amp;"."&amp;$H195</f>
+        <f t="shared" si="6"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K195" s="2" t="s">
@@ -21572,14 +21564,14 @@
         <v>1</v>
       </c>
       <c r="J196" s="2" t="str">
-        <f>$F196&amp;"."&amp;$G196&amp;"."&amp;$H196</f>
+        <f t="shared" si="6"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K196" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="197" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>38</v>
       </c>
@@ -21609,7 +21601,7 @@
         <v>1</v>
       </c>
       <c r="J197" s="2" t="str">
-        <f>$F197&amp;"."&amp;$G197&amp;"."&amp;$H197</f>
+        <f t="shared" si="6"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K197" s="2" t="s">
@@ -21646,14 +21638,14 @@
         <v>1</v>
       </c>
       <c r="J198" s="2" t="str">
-        <f>$F198&amp;"."&amp;$G198&amp;"."&amp;$H198</f>
+        <f t="shared" si="6"/>
         <v>correct.none.yes</v>
       </c>
       <c r="K198" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="199" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>33</v>
       </c>
@@ -21683,14 +21675,14 @@
         <v>4</v>
       </c>
       <c r="J199" s="2" t="str">
-        <f>$F199&amp;"."&amp;$G199&amp;"."&amp;$H199</f>
+        <f t="shared" si="6"/>
         <v>none.none.no</v>
       </c>
       <c r="K199" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="200" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>34</v>
       </c>
@@ -21720,14 +21712,14 @@
         <v>4</v>
       </c>
       <c r="J200" s="2" t="str">
-        <f>$F200&amp;"."&amp;$G200&amp;"."&amp;$H200</f>
+        <f t="shared" si="6"/>
         <v>none.none.no</v>
       </c>
       <c r="K200" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>35</v>
       </c>
@@ -21757,14 +21749,14 @@
         <v>4</v>
       </c>
       <c r="J201" s="2" t="str">
-        <f>$F201&amp;"."&amp;$G201&amp;"."&amp;$H201</f>
+        <f t="shared" si="6"/>
         <v>none.none.no</v>
       </c>
       <c r="K201" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="202" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202" s="14" t="s">
         <v>37</v>
       </c>
@@ -21794,14 +21786,14 @@
         <v>2</v>
       </c>
       <c r="J202" s="14" t="str">
-        <f>$F202&amp;"."&amp;$G202&amp;"."&amp;$H202</f>
+        <f t="shared" si="6"/>
         <v>both.none.no</v>
       </c>
       <c r="K202" s="14" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="203" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>39</v>
       </c>
@@ -21831,7 +21823,7 @@
         <v>2</v>
       </c>
       <c r="J203" s="2" t="str">
-        <f>$F203&amp;"."&amp;$G203&amp;"."&amp;$H203</f>
+        <f t="shared" si="6"/>
         <v>both.none.no</v>
       </c>
       <c r="K203" s="2" t="s">
@@ -21868,14 +21860,14 @@
         <v>2</v>
       </c>
       <c r="J204" s="2" t="str">
-        <f>$F204&amp;"."&amp;$G204&amp;"."&amp;$H204</f>
+        <f t="shared" si="6"/>
         <v>both.none.no</v>
       </c>
       <c r="K204" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>38</v>
       </c>
@@ -21905,21 +21897,21 @@
         <v>2</v>
       </c>
       <c r="J205" s="2" t="str">
-        <f>$F205&amp;"."&amp;$G205&amp;"."&amp;$H205</f>
+        <f t="shared" si="6"/>
         <v>both.none.no</v>
       </c>
       <c r="K205" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="206" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A206" s="65" t="s">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A206" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B206" s="65" t="s">
+      <c r="B206" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C206" s="65" t="s">
+      <c r="C206" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D206" s="57" t="s">
@@ -21928,28 +21920,28 @@
       <c r="E206" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="F206" s="65" t="s">
+      <c r="F206" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G206" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H206" s="65" t="s">
+      <c r="G206" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H206" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I206" s="65">
+      <c r="I206" s="2">
         <f>IFERROR(INT(IF($J206=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J206=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J206=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J206=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J206=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J206=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J206=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J206=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J206=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J206=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J206=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J206=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J206=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J206=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J206=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J206=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J206=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J206=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J206=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J206=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J206=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J206=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J206=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J206=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J206=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J206=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J206=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>2</v>
       </c>
-      <c r="J206" s="65" t="str">
-        <f>$F206&amp;"."&amp;$G206&amp;"."&amp;$H206</f>
+      <c r="J206" s="2" t="str">
+        <f t="shared" si="6"/>
         <v>both.none.no</v>
       </c>
-      <c r="K206" s="65" t="s">
+      <c r="K206" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="207" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
         <v>34</v>
       </c>
@@ -21979,14 +21971,14 @@
         <v>2</v>
       </c>
       <c r="J207" s="2" t="str">
-        <f>$F207&amp;"."&amp;$G207&amp;"."&amp;$H207</f>
+        <f t="shared" si="6"/>
         <v>both.none.no</v>
       </c>
       <c r="K207" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
         <v>35</v>
       </c>
@@ -22016,7 +22008,7 @@
         <v>2</v>
       </c>
       <c r="J208" s="2" t="str">
-        <f>$F208&amp;"."&amp;$G208&amp;"."&amp;$H208</f>
+        <f t="shared" si="6"/>
         <v>both.none.no</v>
       </c>
       <c r="K208" s="2" t="s">
@@ -22060,7 +22052,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="210" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210" s="14" t="s">
         <v>37</v>
       </c>
@@ -22090,14 +22082,14 @@
         <v>2</v>
       </c>
       <c r="J210" s="14" t="str">
-        <f>$F210&amp;"."&amp;$G210&amp;"."&amp;$H210</f>
+        <f t="shared" ref="J210:J217" si="7">$F210&amp;"."&amp;$G210&amp;"."&amp;$H210</f>
         <v>both.none.yes_same</v>
       </c>
       <c r="K210" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
         <v>39</v>
       </c>
@@ -22127,7 +22119,7 @@
         <v>2</v>
       </c>
       <c r="J211" s="2" t="str">
-        <f>$F211&amp;"."&amp;$G211&amp;"."&amp;$H211</f>
+        <f t="shared" si="7"/>
         <v>both.none.yes_same</v>
       </c>
       <c r="K211" s="2" t="s">
@@ -22164,14 +22156,14 @@
         <v>2</v>
       </c>
       <c r="J212" s="2" t="str">
-        <f>$F212&amp;"."&amp;$G212&amp;"."&amp;$H212</f>
+        <f t="shared" si="7"/>
         <v>both.none.yes_same</v>
       </c>
       <c r="K212" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
         <v>38</v>
       </c>
@@ -22201,7 +22193,7 @@
         <v>2</v>
       </c>
       <c r="J213" s="2" t="str">
-        <f>$F213&amp;"."&amp;$G213&amp;"."&amp;$H213</f>
+        <f t="shared" si="7"/>
         <v>both.none.yes_same</v>
       </c>
       <c r="K213" s="2" t="s">
@@ -22209,13 +22201,13 @@
       </c>
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A214" s="65" t="s">
+      <c r="A214" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B214" s="65" t="s">
+      <c r="B214" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C214" s="65" t="s">
+      <c r="C214" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D214" s="57" t="s">
@@ -22224,28 +22216,28 @@
       <c r="E214" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="F214" s="65" t="s">
+      <c r="F214" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G214" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H214" s="65" t="s">
+      <c r="G214" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H214" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I214" s="65">
+      <c r="I214" s="2">
         <f>IFERROR(INT(IF($J214=SecurityRating!$E$2,SecurityRating!$D$2,"")&amp;IF($J214=SecurityRating!$E$3,SecurityRating!$D$3,"")&amp;IF($J214=SecurityRating!$E$4,SecurityRating!$D$4,"")&amp;IF($J214=SecurityRating!$E$5,SecurityRating!$D$5,"")&amp;IF($J214=SecurityRating!$E$6,SecurityRating!$D$6,"")&amp;IF($J214=SecurityRating!$E$7,SecurityRating!$D$7,"")&amp;IF($J214=SecurityRating!$E$8,SecurityRating!$D$8,"")&amp;IF($J214=SecurityRating!$E$9,SecurityRating!$D$9,"")&amp;IF($J214=SecurityRating!$E$10,SecurityRating!$D$10,"")&amp;IF($J214=SecurityRating!$E$11,SecurityRating!$D$11,"")&amp;IF($J214=SecurityRating!$E$12,SecurityRating!$D$12,"")&amp;IF($J214=SecurityRating!$E$13,SecurityRating!$D$13,"")&amp;IF($J214=SecurityRating!$E$14,SecurityRating!$D$14,"")&amp;IF($J214=SecurityRating!$E$15,SecurityRating!$D$15,"")&amp;IF($J214=SecurityRating!$E$16,SecurityRating!$D$16,"")&amp;IF($J214=SecurityRating!$E$17,SecurityRating!$D$17,"")&amp;IF($J214=SecurityRating!$E$18,SecurityRating!$D$18,"")&amp;IF($J214=SecurityRating!$E$19,SecurityRating!$D$19,"")&amp;IF($J214=SecurityRating!$E$20,SecurityRating!$D$20,"")&amp;IF($J214=SecurityRating!$E$21,SecurityRating!$D$21,"")&amp;IF($J214=SecurityRating!$E$22,SecurityRating!$D$22,"")&amp;IF($J214=SecurityRating!$E$23,SecurityRating!$D$23,"")&amp;IF($J214=SecurityRating!$E$24,SecurityRating!$D$24,"")&amp;IF($J214=SecurityRating!$E$25,SecurityRating!$D$25,"")&amp;IF($J214=SecurityRating!$E$26,SecurityRating!$D$26,"")&amp;IF($J214=SecurityRating!$E$27,SecurityRating!$D$27,"")&amp;IF($J214=SecurityRating!$E$28,SecurityRating!$D$28,"")),"")</f>
         <v>2</v>
       </c>
-      <c r="J214" s="65" t="str">
-        <f>$F214&amp;"."&amp;$G214&amp;"."&amp;$H214</f>
+      <c r="J214" s="2" t="str">
+        <f t="shared" si="7"/>
         <v>both.none.yes_same</v>
       </c>
-      <c r="K214" s="65" t="s">
+      <c r="K214" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
         <v>33</v>
       </c>
@@ -22275,14 +22267,14 @@
         <v>4</v>
       </c>
       <c r="J215" s="2" t="str">
-        <f>$F215&amp;"."&amp;$G215&amp;"."&amp;$H215</f>
+        <f t="shared" si="7"/>
         <v>none.none.no</v>
       </c>
       <c r="K215" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
         <v>34</v>
       </c>
@@ -22312,14 +22304,14 @@
         <v>4</v>
       </c>
       <c r="J216" s="2" t="str">
-        <f>$F216&amp;"."&amp;$G216&amp;"."&amp;$H216</f>
+        <f t="shared" si="7"/>
         <v>none.none.no</v>
       </c>
       <c r="K216" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
         <v>35</v>
       </c>
@@ -22349,7 +22341,7 @@
         <v>4</v>
       </c>
       <c r="J217" s="2" t="str">
-        <f>$F217&amp;"."&amp;$G217&amp;"."&amp;$H217</f>
+        <f t="shared" si="7"/>
         <v>none.none.no</v>
       </c>
       <c r="K217" s="2" t="s">

</xml_diff>